<commit_message>
added multiple vBatt reads with average
</commit_message>
<xml_diff>
--- a/ElectricImp_Dice/Imp to MMA8452Q pinout.xlsx
+++ b/ElectricImp_Dice/Imp to MMA8452Q pinout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
   <si>
     <t>Pin 9</t>
   </si>
@@ -112,6 +112,9 @@
   </si>
   <si>
     <t>SDA pin1</t>
+  </si>
+  <si>
+    <t>VBATT</t>
   </si>
 </sst>
 </file>
@@ -514,13 +517,14 @@
   <dimension ref="B3:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
     <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:10" x14ac:dyDescent="0.25">
@@ -591,6 +595,9 @@
       </c>
       <c r="E7">
         <v>5</v>
+      </c>
+      <c r="F7" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">

</xml_diff>